<commit_message>
-- all 5 methods implemented
</commit_message>
<xml_diff>
--- a/pathfinder/expandresults.xlsx
+++ b/pathfinder/expandresults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="900" windowWidth="31760" windowHeight="9720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="expandresults.xls" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -137,7 +137,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -473,10 +473,13 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="R3" sqref="R3:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="1">

</xml_diff>